<commit_message>
Ciclo seriado en agregar consulta mensual para evitar errores. Corrige el template editPatient
</commit_message>
<xml_diff>
--- a/formato.xlsx
+++ b/formato.xlsx
@@ -2100,530 +2100,6 @@
       <c r="BN2" s="2"/>
       <c r="BO2" s="2"/>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K3" t="s">
-        <v>68</v>
-      </c>
-      <c r="L3" t="s">
-        <v>69</v>
-      </c>
-      <c r="M3" t="s">
-        <v>70</v>
-      </c>
-      <c r="N3" t="s">
-        <v>71</v>
-      </c>
-      <c r="O3" t="s">
-        <v>70</v>
-      </c>
-      <c r="P3" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>70</v>
-      </c>
-      <c r="R3" t="s">
-        <v>72</v>
-      </c>
-      <c r="S3" t="s">
-        <v>72</v>
-      </c>
-      <c r="T3" t="s">
-        <v>73</v>
-      </c>
-      <c r="U3" t="s">
-        <v>67</v>
-      </c>
-      <c r="V3" t="s">
-        <v>74</v>
-      </c>
-      <c r="W3" t="s">
-        <v>75</v>
-      </c>
-      <c r="X3" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>80</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I4" t="s">
-        <v>85</v>
-      </c>
-      <c r="J4" t="s">
-        <v>86</v>
-      </c>
-      <c r="K4" t="s">
-        <v>68</v>
-      </c>
-      <c r="L4" t="s">
-        <v>69</v>
-      </c>
-      <c r="M4" t="s">
-        <v>70</v>
-      </c>
-      <c r="N4" t="s">
-        <v>71</v>
-      </c>
-      <c r="O4" t="s">
-        <v>83</v>
-      </c>
-      <c r="P4" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>70</v>
-      </c>
-      <c r="R4" t="s">
-        <v>72</v>
-      </c>
-      <c r="S4" t="s">
-        <v>72</v>
-      </c>
-      <c r="T4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U4" t="s">
-        <v>86</v>
-      </c>
-      <c r="V4" t="s">
-        <v>74</v>
-      </c>
-      <c r="W4" t="s">
-        <v>75</v>
-      </c>
-      <c r="X4" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>86</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>74</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" t="s">
-        <v>84</v>
-      </c>
-      <c r="I5" t="s">
-        <v>88</v>
-      </c>
-      <c r="J5" t="s">
-        <v>89</v>
-      </c>
-      <c r="K5" t="s">
-        <v>68</v>
-      </c>
-      <c r="L5" t="s">
-        <v>73</v>
-      </c>
-      <c r="M5" t="s">
-        <v>70</v>
-      </c>
-      <c r="N5" t="s">
-        <v>71</v>
-      </c>
-      <c r="O5" t="s">
-        <v>83</v>
-      </c>
-      <c r="P5" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>70</v>
-      </c>
-      <c r="R5" t="s">
-        <v>79</v>
-      </c>
-      <c r="S5" t="s">
-        <v>67</v>
-      </c>
-      <c r="T5" t="s">
-        <v>74</v>
-      </c>
-      <c r="U5" t="s">
-        <v>91</v>
-      </c>
-      <c r="V5" t="s">
-        <v>74</v>
-      </c>
-      <c r="W5" t="s">
-        <v>75</v>
-      </c>
-      <c r="X5" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>74</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>65</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>77</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G6" t="s">
-        <v>99</v>
-      </c>
-      <c r="H6" t="s">
-        <v>55</v>
-      </c>
-      <c r="I6" t="s">
-        <v>100</v>
-      </c>
-      <c r="J6" t="s">
-        <v>101</v>
-      </c>
-      <c r="K6" t="s">
-        <v>68</v>
-      </c>
-      <c r="L6" t="s">
-        <v>73</v>
-      </c>
-      <c r="M6" t="s">
-        <v>70</v>
-      </c>
-      <c r="N6" t="s">
-        <v>71</v>
-      </c>
-      <c r="O6" t="s">
-        <v>83</v>
-      </c>
-      <c r="P6" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>70</v>
-      </c>
-      <c r="R6" t="s">
-        <v>72</v>
-      </c>
-      <c r="S6" t="s">
-        <v>72</v>
-      </c>
-      <c r="T6" t="s">
-        <v>67</v>
-      </c>
-      <c r="U6" t="s">
-        <v>89</v>
-      </c>
-      <c r="V6" t="s">
-        <v>74</v>
-      </c>
-      <c r="W6" t="s">
-        <v>75</v>
-      </c>
-      <c r="X6" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>93</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>101</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>74</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>65</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>77</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>81</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>70</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:I1"/>

</xml_diff>

<commit_message>
Agregamos las columnas de consulta mensual 1 al excel.
</commit_message>
<xml_diff>
--- a/formato.xlsx
+++ b/formato.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar\Desktop\AdminControl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Downloads/AdminControl/AdminControl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393052BD-2E27-40BA-B5A1-BA4B7565D02D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFC1A34-C451-B940-BC5B-AEE763C77236}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4900" yWindow="4900" windowWidth="28800" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1100" windowWidth="28800" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expediente" sheetId="1" r:id="rId1"/>
@@ -233,7 +233,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>Nombre</t>
   </si>
@@ -370,183 +370,98 @@
     <t>Translocación (14;16)</t>
   </si>
   <si>
-    <t>Romina Chavez Hurtado</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>1978-05-09</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>2011-05-17</t>
-  </si>
-  <si>
-    <t>170</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>1.86 m²</t>
-  </si>
-  <si>
-    <t>68</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Si</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
     <t>IgA</t>
   </si>
   <si>
-    <t>Kappa</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>58</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>2019-04-01</t>
-  </si>
-  <si>
-    <t>250</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Neumonia</t>
-  </si>
-  <si>
-    <t>ninguna</t>
-  </si>
-  <si>
-    <t>2019-04-08</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>Urinaria</t>
-  </si>
-  <si>
-    <t>ninguna3</t>
-  </si>
-  <si>
-    <t>Ariel Solis Ruiz</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>1979-10-18</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>2018-04-02</t>
-  </si>
-  <si>
-    <t>180</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>1.87 m²</t>
-  </si>
-  <si>
     <t>IgG</t>
   </si>
   <si>
-    <t>74</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>2019-06-01</t>
-  </si>
-  <si>
-    <t>Lambda</t>
-  </si>
-  <si>
-    <t>EE</t>
-  </si>
-  <si>
-    <t>prueba final</t>
+    <t>CONSULTA MENSUAL 1</t>
+  </si>
+  <si>
+    <t>Ciclo de Tratamiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha de realización </t>
+  </si>
+  <si>
+    <t>Albumina</t>
+  </si>
+  <si>
+    <t>Calcio Sérico</t>
+  </si>
+  <si>
+    <t>Deshidrogenasa Láctica</t>
+  </si>
+  <si>
+    <t>Hemoglobina</t>
+  </si>
+  <si>
+    <t>Hematocrito</t>
+  </si>
+  <si>
+    <t>Leucocitos</t>
+  </si>
+  <si>
+    <t>Linfocitos</t>
+  </si>
+  <si>
+    <t>Neutrofilos</t>
+  </si>
+  <si>
+    <t>Plaquetas</t>
+  </si>
+  <si>
+    <t>IgM</t>
+  </si>
+  <si>
+    <t>Cadenas Ligeras Kappa</t>
+  </si>
+  <si>
+    <t>Cadenas Ligeras Lambda</t>
+  </si>
+  <si>
+    <t>Toxicidad Hematológica - Serie Roja</t>
+  </si>
+  <si>
+    <t>Toxicidad Hematológica - Neutrofilos</t>
+  </si>
+  <si>
+    <t>Toxicidad Hematológica - Plaquetas</t>
+  </si>
+  <si>
+    <t>Toxicidad Hepática</t>
+  </si>
+  <si>
+    <t>Toxicidad Renal</t>
+  </si>
+  <si>
+    <t>Toxicidad Gastrointestinal-Nausea</t>
+  </si>
+  <si>
+    <t>Toxicidad Gastrointestinal-Diarrea</t>
+  </si>
+  <si>
+    <t>Toxicidad neuropatía periférica</t>
+  </si>
+  <si>
+    <t>Toxicidad Infecciosa</t>
+  </si>
+  <si>
+    <t>Sitio de infección</t>
+  </si>
+  <si>
+    <t>Reacción a infusión de medicamentos</t>
+  </si>
+  <si>
+    <t>Reacción adversa otra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -903,51 +818,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BO4"/>
+  <dimension ref="A1:CB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="AX1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BH5" sqref="BH5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="41.08203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="18.0" collapsed="true"/>
-    <col min="4" max="9" customWidth="true" style="5" width="18.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="5" width="20.75" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.1640625" collapsed="true"/>
-    <col min="13" max="14" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="15" max="17" customWidth="true" width="27.1640625" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="29.33203125" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="32.75" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="13.5" collapsed="true"/>
-    <col min="21" max="26" customWidth="true" width="27.1640625" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="33.6640625" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" width="33.1640625" collapsed="true"/>
-    <col min="29" max="43" customWidth="true" width="27.1640625" collapsed="true"/>
-    <col min="44" max="44" customWidth="true" width="15.5" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="5.6640625" collapsed="true"/>
-    <col min="46" max="46" customWidth="true" width="8.1640625" collapsed="true"/>
-    <col min="47" max="47" customWidth="true" width="8.5" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="9.6640625" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="8.83203125" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="10.1640625" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="52" max="52" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="13.5" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="13.5" collapsed="true"/>
-    <col min="56" max="56" customWidth="true" width="13.5" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="13.83203125" collapsed="true"/>
-    <col min="58" max="58" customWidth="true" width="13.83203125" collapsed="true"/>
-    <col min="61" max="61" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="66" max="66" customWidth="true" width="21.1640625" collapsed="true"/>
-    <col min="67" max="67" customWidth="true" width="20.5" collapsed="true"/>
+    <col min="1" max="1" width="41" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="9" width="18" style="5" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.6640625" style="5" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="14" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="17" width="27.1640625" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="29.33203125" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="32.6640625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.5" customWidth="1" collapsed="1"/>
+    <col min="21" max="26" width="27.1640625" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="33.6640625" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="33.1640625" customWidth="1" collapsed="1"/>
+    <col min="29" max="43" width="27.1640625" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="19.83203125" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="27.33203125" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="18.83203125" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="18.5" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="20.5" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="15.5" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="15.1640625" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="15.5" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="9" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="13.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="13.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="13.5" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="13.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="22" customWidth="1"/>
+    <col min="59" max="59" width="21.83203125" customWidth="1"/>
+    <col min="60" max="60" width="30.6640625" customWidth="1"/>
+    <col min="61" max="61" width="33" customWidth="1"/>
+    <col min="62" max="62" width="31" customWidth="1"/>
+    <col min="63" max="63" width="19.5" customWidth="1"/>
+    <col min="64" max="64" width="16.5" customWidth="1"/>
+    <col min="65" max="65" width="30.33203125" customWidth="1"/>
+    <col min="66" max="66" width="30.6640625" customWidth="1"/>
+    <col min="67" max="67" width="27.6640625" customWidth="1"/>
+    <col min="68" max="68" width="27.33203125" customWidth="1"/>
+    <col min="69" max="69" width="26.83203125" customWidth="1"/>
+    <col min="70" max="70" width="32.33203125" customWidth="1"/>
+    <col min="71" max="71" width="27.6640625" customWidth="1"/>
+    <col min="72" max="72" width="24.6640625" customWidth="1"/>
+    <col min="74" max="74" width="9" customWidth="1" collapsed="1"/>
+    <col min="79" max="79" width="21.1640625" customWidth="1" collapsed="1"/>
+    <col min="80" max="80" width="20.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
@@ -995,7 +924,9 @@
       <c r="AO1" s="8"/>
       <c r="AP1" s="8"/>
       <c r="AQ1" s="8"/>
-      <c r="AR1" s="9"/>
+      <c r="AR1" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="AS1" s="9"/>
       <c r="AT1" s="9"/>
       <c r="AU1" s="9"/>
@@ -1010,17 +941,30 @@
       <c r="BD1" s="9"/>
       <c r="BE1" s="9"/>
       <c r="BF1" s="9"/>
-      <c r="BG1" s="7"/>
-      <c r="BH1" s="7"/>
-      <c r="BI1" s="7"/>
-      <c r="BJ1" s="7"/>
-      <c r="BK1" s="7"/>
-      <c r="BL1" s="7"/>
-      <c r="BM1" s="8"/>
-      <c r="BN1" s="8"/>
-      <c r="BO1" s="8"/>
+      <c r="BG1" s="9"/>
+      <c r="BH1" s="9"/>
+      <c r="BI1" s="9"/>
+      <c r="BJ1" s="9"/>
+      <c r="BK1" s="9"/>
+      <c r="BL1" s="9"/>
+      <c r="BM1" s="9"/>
+      <c r="BN1" s="9"/>
+      <c r="BO1" s="9"/>
+      <c r="BP1" s="9"/>
+      <c r="BQ1" s="9"/>
+      <c r="BR1" s="9"/>
+      <c r="BS1" s="9"/>
+      <c r="BT1" s="7"/>
+      <c r="BU1" s="7"/>
+      <c r="BV1" s="7"/>
+      <c r="BW1" s="7"/>
+      <c r="BX1" s="7"/>
+      <c r="BY1" s="7"/>
+      <c r="BZ1" s="8"/>
+      <c r="CA1" s="8"/>
+      <c r="CB1" s="8"/>
     </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1150,546 +1094,107 @@
       <c r="AQ2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AR2" s="3"/>
-      <c r="AS2" s="3"/>
-      <c r="AT2" s="3"/>
-      <c r="AU2" s="3"/>
-      <c r="AV2" s="3"/>
-      <c r="AW2" s="3"/>
-      <c r="AX2" s="3"/>
-      <c r="AY2" s="3"/>
-      <c r="AZ2" s="3"/>
-      <c r="BA2" s="3"/>
-      <c r="BB2" s="3"/>
-      <c r="BC2" s="3"/>
-      <c r="BD2" s="3"/>
-      <c r="BE2" s="3"/>
-      <c r="BF2" s="3"/>
-      <c r="BG2" s="1"/>
-      <c r="BH2" s="1"/>
-      <c r="BI2" s="1"/>
-      <c r="BJ2" s="1"/>
-      <c r="BK2" s="1"/>
-      <c r="BL2" s="1"/>
-      <c r="BM2" s="2"/>
-      <c r="BN2" s="2"/>
-      <c r="BO2" s="2"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="AR2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AY2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="BD2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" t="s">
-        <v>54</v>
-      </c>
-      <c r="K3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L3" t="s">
-        <v>56</v>
-      </c>
-      <c r="M3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N3" t="s">
-        <v>58</v>
-      </c>
-      <c r="O3" t="s">
-        <v>57</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="BE2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="BF2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="R3" t="s">
+      <c r="BG2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="S3" t="s">
-        <v>61</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="BH2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="U3" t="s">
-        <v>56</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="BI2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="W3" t="s">
+      <c r="BJ2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="X3" t="s">
+      <c r="BK2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="Y3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z3" t="s">
+      <c r="BL2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AA3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB3" t="s">
+      <c r="BM2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="AC3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF3" t="s">
+      <c r="BN2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="AG3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AH3" t="s">
+      <c r="BO2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AI3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AM3" t="s">
+      <c r="BP2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="AN3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS3" t="s">
+      <c r="BQ2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AT3" t="s">
+      <c r="BR2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="AU3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AV3" t="s">
+      <c r="BS2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AW3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>76</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>62</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>75</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>77</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>56</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>76</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>58</v>
-      </c>
-      <c r="BI3" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>78</v>
-      </c>
-      <c r="BK3" t="s">
-        <v>79</v>
-      </c>
-      <c r="BL3" t="s">
-        <v>78</v>
-      </c>
-      <c r="BM3" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN3" t="s">
-        <v>77</v>
-      </c>
-      <c r="BO3" t="s">
-        <v>78</v>
-      </c>
-      <c r="BP3" t="s">
-        <v>80</v>
-      </c>
-      <c r="BQ3" t="s">
-        <v>56</v>
-      </c>
-      <c r="BR3" t="s">
-        <v>81</v>
-      </c>
-      <c r="BS3" t="s">
-        <v>56</v>
-      </c>
-      <c r="BT3" t="s">
-        <v>82</v>
-      </c>
-      <c r="BU3" t="s">
-        <v>83</v>
-      </c>
-      <c r="BV3" t="s">
-        <v>55</v>
-      </c>
-      <c r="BW3" t="s">
-        <v>61</v>
-      </c>
-      <c r="BX3" t="s">
-        <v>74</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>55</v>
-      </c>
-      <c r="BZ3" t="s">
-        <v>61</v>
-      </c>
-      <c r="CA3" t="s">
-        <v>76</v>
-      </c>
-      <c r="CB3" t="s">
-        <v>61</v>
-      </c>
-      <c r="CC3" t="s">
-        <v>84</v>
-      </c>
-      <c r="CD3" t="s">
-        <v>67</v>
-      </c>
-      <c r="CE3" t="s">
-        <v>59</v>
-      </c>
-      <c r="CF3" t="s">
-        <v>76</v>
-      </c>
-      <c r="CG3" t="s">
-        <v>84</v>
-      </c>
-      <c r="CH3" t="s">
-        <v>84</v>
-      </c>
-      <c r="CI3" t="s">
-        <v>78</v>
-      </c>
-      <c r="CJ3" t="s">
-        <v>77</v>
-      </c>
-      <c r="CK3" t="s">
-        <v>77</v>
-      </c>
-      <c r="CL3" t="s">
-        <v>78</v>
-      </c>
-      <c r="CM3" t="s">
-        <v>58</v>
-      </c>
-      <c r="CN3" t="s">
-        <v>56</v>
-      </c>
-      <c r="CO3" t="s">
-        <v>58</v>
-      </c>
-      <c r="CP3" t="s">
-        <v>78</v>
-      </c>
-      <c r="CQ3" t="s">
-        <v>85</v>
-      </c>
-      <c r="CR3" t="s">
-        <v>79</v>
-      </c>
-      <c r="CS3" t="s">
-        <v>86</v>
-      </c>
-      <c r="CT3"/>
-      <c r="IZ3" t="s">
-        <v>98</v>
-      </c>
-      <c r="JA3" t="s">
-        <v>79</v>
-      </c>
-      <c r="JB3" t="s">
-        <v>59</v>
-      </c>
-      <c r="JC3" t="s">
-        <v>61</v>
-      </c>
-      <c r="JD3" t="s">
-        <v>76</v>
-      </c>
-      <c r="JE3" t="s">
-        <v>62</v>
-      </c>
-      <c r="JF3" t="s">
-        <v>96</v>
-      </c>
-      <c r="JG3" t="s">
-        <v>62</v>
-      </c>
-      <c r="JH3" t="s">
-        <v>97</v>
-      </c>
-      <c r="JI3" t="s">
-        <v>62</v>
-      </c>
-      <c r="JJ3" t="s">
-        <v>79</v>
-      </c>
-      <c r="JK3" t="s">
-        <v>75</v>
-      </c>
-      <c r="JL3" t="s">
-        <v>61</v>
-      </c>
-      <c r="JM3" t="s">
-        <v>56</v>
-      </c>
-      <c r="JN3" t="s">
-        <v>84</v>
-      </c>
-      <c r="JO3" t="s">
-        <v>56</v>
-      </c>
-      <c r="JP3" t="s">
-        <v>73</v>
-      </c>
-      <c r="JQ3" t="s">
-        <v>59</v>
-      </c>
-      <c r="JR3" t="s">
-        <v>64</v>
-      </c>
-      <c r="JS3" t="s">
-        <v>99</v>
-      </c>
-      <c r="JT3" t="s">
-        <v>84</v>
-      </c>
-      <c r="JU3" t="s">
-        <v>100</v>
-      </c>
-      <c r="JV3" t="s">
-        <v>101</v>
-      </c>
-      <c r="JW3"/>
-      <c r="JX3"/>
-      <c r="JY3"/>
-      <c r="JZ3"/>
-      <c r="KA3"/>
-      <c r="KB3"/>
-      <c r="KC3"/>
-      <c r="KD3"/>
-      <c r="KE3"/>
-      <c r="KF3"/>
-      <c r="KG3"/>
-      <c r="KH3"/>
-      <c r="KI3"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G4" t="s">
-        <v>93</v>
-      </c>
-      <c r="H4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" t="s">
-        <v>94</v>
-      </c>
-      <c r="J4" t="s">
-        <v>84</v>
-      </c>
-      <c r="K4" t="s">
-        <v>59</v>
-      </c>
-      <c r="L4" t="s">
-        <v>56</v>
-      </c>
-      <c r="M4" t="s">
-        <v>57</v>
-      </c>
-      <c r="N4" t="s">
-        <v>58</v>
-      </c>
-      <c r="O4" t="s">
-        <v>57</v>
-      </c>
-      <c r="P4" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>60</v>
-      </c>
-      <c r="R4" t="s">
-        <v>61</v>
-      </c>
-      <c r="S4" t="s">
-        <v>61</v>
-      </c>
-      <c r="T4" t="s">
-        <v>59</v>
-      </c>
-      <c r="U4" t="s">
-        <v>84</v>
-      </c>
-      <c r="V4" t="s">
-        <v>61</v>
-      </c>
-      <c r="W4" t="s">
-        <v>95</v>
-      </c>
-      <c r="X4" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>96</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>97</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>60</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>60</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>60</v>
-      </c>
-      <c r="AR4"/>
+      <c r="BT2" s="1"/>
+      <c r="BU2" s="1"/>
+      <c r="BV2" s="1"/>
+      <c r="BW2" s="1"/>
+      <c r="BX2" s="1"/>
+      <c r="BY2" s="1"/>
+      <c r="BZ2" s="2"/>
+      <c r="CA2" s="2"/>
+      <c r="CB2" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="J1:AQ1"/>
-    <mergeCell ref="AR1:BF1"/>
-    <mergeCell ref="BG1:BL1"/>
-    <mergeCell ref="BM1:BO1"/>
+    <mergeCell ref="AR1:BS1"/>
+    <mergeCell ref="BT1:BY1"/>
+    <mergeCell ref="BZ1:CB1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Parte 1 corrección doctora
</commit_message>
<xml_diff>
--- a/formato.xlsx
+++ b/formato.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar\Desktop\AdminControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF90AC68-69F2-42A2-BFB4-A6761ADDB64C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E25D9AE8-31DD-4F2D-926F-565C2B5C45C3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23480" yWindow="4200" windowWidth="28800" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expediente" sheetId="1" r:id="rId1"/>
@@ -24,216 +24,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Microsoft Office User</author>
-  </authors>
-  <commentList>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{650036DB-CC6F-8248-A0C5-50EF850FFCB4}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>DD/MM/AA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{92129247-F582-6046-8DBF-626A2D1D5D40}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Presencia de arritmia CONTROLADA (arritmia no controlada es criterio de exclusiòn):
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Si
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>No</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{07140894-C7E3-D941-A86E-32906EBC7BAC}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Cardiopatía  I o II de NYHA (estadio III o IV es criterio de exclusión):
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Si
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>No</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{977EECDE-FF57-2E4D-92C7-5D5FF9233F1E}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Antecedente de neumopatía crónica controlada/incipiente:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Si
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>No</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{9D295B6D-25E7-9A45-B64C-DB2514006393}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Presencia de hepatopatía crónica compensada/incipiente:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Si
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>No</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="154">
   <si>
     <t>Nombre</t>
   </si>
@@ -515,32 +307,200 @@
   </si>
   <si>
     <t>Reacción Adversa otra</t>
+  </si>
+  <si>
+    <t>Romina Chavez Hurtado</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>1978-05-09</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>2011-05-17</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>1.86 m²</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Kappa</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>2019-04-01</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Neumonia</t>
+  </si>
+  <si>
+    <t>ninguna</t>
+  </si>
+  <si>
+    <t>2019-04-08</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Urinaria</t>
+  </si>
+  <si>
+    <t>ninguna3</t>
+  </si>
+  <si>
+    <t>2019-06-01</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Lambda</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>prueba final</t>
+  </si>
+  <si>
+    <t>Ariel Solis Ruiz</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>1979-10-18</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>2018-04-02</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>1.87 m²</t>
+  </si>
+  <si>
+    <t>Calcio Sérico (mg/dL)</t>
+  </si>
+  <si>
+    <t>Deshidrogenasa Láctica (U/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linfocitos (cels x 10(3)/uL) </t>
+  </si>
+  <si>
+    <t>Cadenas Ligeras Kappa (mg/dL)</t>
+  </si>
+  <si>
+    <t>Cadenas Ligeras Lambda (mg/dL)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -594,7 +554,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -602,27 +562,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -632,8 +577,14 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -643,24 +594,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -945,172 +890,172 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:KQ2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:KQ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="JZ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="IW8" sqref="IW8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="9" width="18" style="5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.6640625" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="17" width="27.1640625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="29.33203125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="13.5" customWidth="1" collapsed="1"/>
-    <col min="21" max="26" width="27.1640625" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="33.6640625" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="33.1640625" customWidth="1" collapsed="1"/>
-    <col min="29" max="43" width="27.1640625" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="19.83203125" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="27.33203125" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="18.83203125" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="18.5" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="20.5" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="15.5" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="15.1640625" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="15.5" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="9" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="13.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="13.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="13.5" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="13.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="22" customWidth="1"/>
-    <col min="59" max="59" width="21.83203125" customWidth="1"/>
-    <col min="60" max="60" width="30.6640625" customWidth="1"/>
-    <col min="61" max="61" width="33" customWidth="1"/>
-    <col min="62" max="62" width="31" customWidth="1"/>
-    <col min="63" max="63" width="19.5" customWidth="1"/>
-    <col min="64" max="64" width="16.5" customWidth="1"/>
-    <col min="65" max="65" width="30.33203125" customWidth="1"/>
-    <col min="66" max="66" width="30.6640625" customWidth="1"/>
-    <col min="67" max="67" width="27.6640625" customWidth="1"/>
-    <col min="68" max="68" width="27.33203125" customWidth="1"/>
-    <col min="69" max="69" width="26.83203125" customWidth="1"/>
-    <col min="70" max="70" width="32.58203125" customWidth="1"/>
-    <col min="71" max="71" width="32.33203125" customWidth="1"/>
-    <col min="72" max="72" width="20.75" customWidth="1"/>
-    <col min="73" max="73" width="16.9140625" customWidth="1"/>
-    <col min="97" max="97" width="15.5" customWidth="1"/>
-    <col min="98" max="98" width="32.9140625" customWidth="1"/>
-    <col min="99" max="99" width="29.9140625" customWidth="1"/>
-    <col min="126" max="126" width="32.33203125" customWidth="1"/>
-    <col min="127" max="127" width="31.83203125" customWidth="1"/>
-    <col min="153" max="153" width="18.08203125" customWidth="1"/>
-    <col min="154" max="154" width="32.4140625" customWidth="1"/>
-    <col min="155" max="155" width="33" customWidth="1"/>
-    <col min="182" max="182" width="32.08203125" customWidth="1"/>
-    <col min="183" max="183" width="35" customWidth="1"/>
-    <col min="210" max="210" width="32.4140625" customWidth="1"/>
-    <col min="211" max="211" width="32" customWidth="1"/>
-    <col min="237" max="237" width="14.83203125" customWidth="1"/>
-    <col min="238" max="238" width="33.4140625" customWidth="1"/>
-    <col min="239" max="239" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="266" max="266" width="33.58203125" customWidth="1"/>
-    <col min="267" max="267" width="32.33203125" customWidth="1"/>
-    <col min="268" max="268" width="17.9140625" customWidth="1"/>
-    <col min="281" max="281" width="20.9140625" customWidth="1"/>
-    <col min="282" max="282" width="22.6640625" customWidth="1"/>
-    <col min="283" max="294" width="30.9140625" customWidth="1"/>
-    <col min="295" max="295" width="30.6640625" customWidth="1"/>
-    <col min="296" max="296" width="32" customWidth="1"/>
-    <col min="297" max="297" width="33" customWidth="1"/>
-    <col min="298" max="298" width="22.33203125" customWidth="1"/>
-    <col min="299" max="299" width="15.33203125" customWidth="1"/>
-    <col min="300" max="300" width="29.08203125" customWidth="1"/>
-    <col min="301" max="301" width="31" customWidth="1"/>
-    <col min="302" max="302" width="28.4140625" customWidth="1"/>
-    <col min="303" max="303" width="20.25" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="41.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="18.0" collapsed="true"/>
+    <col min="4" max="9" customWidth="true" style="5" width="18.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="20.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="19.1640625" collapsed="true"/>
+    <col min="13" max="14" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="15" max="17" customWidth="true" width="27.1640625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="29.33203125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="13.5" collapsed="true"/>
+    <col min="21" max="26" customWidth="true" width="27.1640625" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="33.6640625" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="33.1640625" collapsed="true"/>
+    <col min="29" max="43" customWidth="true" width="27.1640625" collapsed="true"/>
+    <col min="44" max="44" customWidth="true" width="19.83203125" collapsed="true"/>
+    <col min="45" max="45" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" width="18.5" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" width="28.58203125" collapsed="true"/>
+    <col min="49" max="49" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="50" max="50" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="51" max="51" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="52" max="52" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="13.5" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="55" max="55" bestFit="true" customWidth="true" width="13.5" collapsed="true"/>
+    <col min="56" max="56" customWidth="true" width="13.5" collapsed="true"/>
+    <col min="57" max="57" bestFit="true" customWidth="true" width="13.83203125" collapsed="true"/>
+    <col min="58" max="58" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="59" max="59" customWidth="true" width="21.83203125" collapsed="true"/>
+    <col min="60" max="60" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="61" max="61" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="62" max="62" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="63" max="63" customWidth="true" width="19.5" collapsed="true"/>
+    <col min="64" max="64" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="65" max="65" customWidth="true" width="30.33203125" collapsed="true"/>
+    <col min="66" max="66" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="67" max="67" customWidth="true" width="27.6640625" collapsed="true"/>
+    <col min="68" max="68" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="69" max="69" customWidth="true" width="26.83203125" collapsed="true"/>
+    <col min="70" max="70" customWidth="true" width="32.58203125" collapsed="true"/>
+    <col min="71" max="71" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="72" max="72" customWidth="true" width="20.75" collapsed="true"/>
+    <col min="73" max="73" customWidth="true" width="16.9140625" collapsed="true"/>
+    <col min="97" max="97" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="98" max="98" customWidth="true" width="32.9140625" collapsed="true"/>
+    <col min="99" max="99" customWidth="true" width="29.9140625" collapsed="true"/>
+    <col min="126" max="126" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="127" max="127" customWidth="true" width="31.83203125" collapsed="true"/>
+    <col min="153" max="153" customWidth="true" width="18.08203125" collapsed="true"/>
+    <col min="154" max="154" customWidth="true" width="32.4140625" collapsed="true"/>
+    <col min="155" max="155" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="182" max="182" customWidth="true" width="32.08203125" collapsed="true"/>
+    <col min="183" max="183" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="210" max="210" customWidth="true" width="32.4140625" collapsed="true"/>
+    <col min="211" max="211" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="237" max="237" customWidth="true" width="14.83203125" collapsed="true"/>
+    <col min="238" max="238" customWidth="true" width="33.4140625" collapsed="true"/>
+    <col min="239" max="239" bestFit="true" customWidth="true" width="32.5" collapsed="true"/>
+    <col min="266" max="266" customWidth="true" width="33.58203125" collapsed="true"/>
+    <col min="267" max="267" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="268" max="268" customWidth="true" width="17.9140625" collapsed="true"/>
+    <col min="281" max="281" customWidth="true" width="20.9140625" collapsed="true"/>
+    <col min="282" max="282" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="283" max="294" customWidth="true" width="30.9140625" collapsed="true"/>
+    <col min="295" max="295" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="296" max="296" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="297" max="297" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="298" max="298" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="299" max="299" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="300" max="300" customWidth="true" width="29.08203125" collapsed="true"/>
+    <col min="301" max="301" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="302" max="302" customWidth="true" width="28.4140625" collapsed="true"/>
+    <col min="303" max="303" customWidth="true" width="20.25" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:303" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="10" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10"/>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10"/>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10"/>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="11" t="s">
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="AS1" s="11"/>
-      <c r="AT1" s="11"/>
-      <c r="AU1" s="11"/>
-      <c r="AV1" s="11"/>
-      <c r="AW1" s="11"/>
-      <c r="AX1" s="11"/>
-      <c r="AY1" s="11"/>
-      <c r="AZ1" s="11"/>
-      <c r="BA1" s="11"/>
-      <c r="BB1" s="11"/>
-      <c r="BC1" s="11"/>
-      <c r="BD1" s="11"/>
-      <c r="BE1" s="11"/>
-      <c r="BF1" s="11"/>
-      <c r="BG1" s="11"/>
-      <c r="BH1" s="11"/>
-      <c r="BI1" s="11"/>
-      <c r="BJ1" s="11"/>
-      <c r="BK1" s="11"/>
-      <c r="BL1" s="11"/>
-      <c r="BM1" s="11"/>
-      <c r="BN1" s="11"/>
-      <c r="BO1" s="11"/>
-      <c r="BP1" s="11"/>
-      <c r="BQ1" s="11"/>
-      <c r="BR1" s="11"/>
-      <c r="BS1" s="11"/>
-      <c r="BT1" s="16" t="s">
+      <c r="AS1" s="13"/>
+      <c r="AT1" s="13"/>
+      <c r="AU1" s="13"/>
+      <c r="AV1" s="13"/>
+      <c r="AW1" s="13"/>
+      <c r="AX1" s="13"/>
+      <c r="AY1" s="13"/>
+      <c r="AZ1" s="13"/>
+      <c r="BA1" s="13"/>
+      <c r="BB1" s="13"/>
+      <c r="BC1" s="13"/>
+      <c r="BD1" s="13"/>
+      <c r="BE1" s="13"/>
+      <c r="BF1" s="13"/>
+      <c r="BG1" s="13"/>
+      <c r="BH1" s="13"/>
+      <c r="BI1" s="13"/>
+      <c r="BJ1" s="13"/>
+      <c r="BK1" s="13"/>
+      <c r="BL1" s="13"/>
+      <c r="BM1" s="13"/>
+      <c r="BN1" s="13"/>
+      <c r="BO1" s="13"/>
+      <c r="BP1" s="13"/>
+      <c r="BQ1" s="13"/>
+      <c r="BR1" s="13"/>
+      <c r="BS1" s="13"/>
+      <c r="BT1" s="19" t="s">
         <v>73</v>
       </c>
       <c r="BU1" s="14"/>
@@ -1140,37 +1085,37 @@
       <c r="CS1" s="14"/>
       <c r="CT1" s="14"/>
       <c r="CU1" s="14"/>
-      <c r="CV1" s="19" t="s">
+      <c r="CV1" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="CW1" s="17"/>
-      <c r="CX1" s="17"/>
-      <c r="CY1" s="17"/>
-      <c r="CZ1" s="17"/>
-      <c r="DA1" s="17"/>
-      <c r="DB1" s="17"/>
-      <c r="DC1" s="17"/>
-      <c r="DD1" s="17"/>
-      <c r="DE1" s="17"/>
-      <c r="DF1" s="17"/>
-      <c r="DG1" s="17"/>
-      <c r="DH1" s="17"/>
-      <c r="DI1" s="17"/>
-      <c r="DJ1" s="17"/>
-      <c r="DK1" s="17"/>
-      <c r="DL1" s="17"/>
-      <c r="DM1" s="17"/>
-      <c r="DN1" s="17"/>
-      <c r="DO1" s="17"/>
-      <c r="DP1" s="17"/>
-      <c r="DQ1" s="17"/>
-      <c r="DR1" s="17"/>
-      <c r="DS1" s="17"/>
-      <c r="DT1" s="17"/>
-      <c r="DU1" s="17"/>
-      <c r="DV1" s="17"/>
-      <c r="DW1" s="17"/>
-      <c r="DX1" s="16" t="s">
+      <c r="CW1" s="16"/>
+      <c r="CX1" s="16"/>
+      <c r="CY1" s="16"/>
+      <c r="CZ1" s="16"/>
+      <c r="DA1" s="16"/>
+      <c r="DB1" s="16"/>
+      <c r="DC1" s="16"/>
+      <c r="DD1" s="16"/>
+      <c r="DE1" s="16"/>
+      <c r="DF1" s="16"/>
+      <c r="DG1" s="16"/>
+      <c r="DH1" s="16"/>
+      <c r="DI1" s="16"/>
+      <c r="DJ1" s="16"/>
+      <c r="DK1" s="16"/>
+      <c r="DL1" s="16"/>
+      <c r="DM1" s="16"/>
+      <c r="DN1" s="16"/>
+      <c r="DO1" s="16"/>
+      <c r="DP1" s="16"/>
+      <c r="DQ1" s="16"/>
+      <c r="DR1" s="16"/>
+      <c r="DS1" s="16"/>
+      <c r="DT1" s="16"/>
+      <c r="DU1" s="16"/>
+      <c r="DV1" s="16"/>
+      <c r="DW1" s="16"/>
+      <c r="DX1" s="19" t="s">
         <v>75</v>
       </c>
       <c r="DY1" s="14"/>
@@ -1200,37 +1145,37 @@
       <c r="EW1" s="14"/>
       <c r="EX1" s="14"/>
       <c r="EY1" s="14"/>
-      <c r="EZ1" s="19" t="s">
+      <c r="EZ1" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="FA1" s="17"/>
-      <c r="FB1" s="17"/>
-      <c r="FC1" s="17"/>
-      <c r="FD1" s="17"/>
-      <c r="FE1" s="17"/>
-      <c r="FF1" s="17"/>
-      <c r="FG1" s="17"/>
-      <c r="FH1" s="17"/>
-      <c r="FI1" s="17"/>
-      <c r="FJ1" s="17"/>
-      <c r="FK1" s="17"/>
-      <c r="FL1" s="17"/>
-      <c r="FM1" s="17"/>
-      <c r="FN1" s="17"/>
-      <c r="FO1" s="17"/>
-      <c r="FP1" s="17"/>
-      <c r="FQ1" s="17"/>
-      <c r="FR1" s="17"/>
-      <c r="FS1" s="17"/>
-      <c r="FT1" s="17"/>
-      <c r="FU1" s="17"/>
-      <c r="FV1" s="17"/>
-      <c r="FW1" s="17"/>
-      <c r="FX1" s="17"/>
-      <c r="FY1" s="17"/>
-      <c r="FZ1" s="17"/>
-      <c r="GA1" s="17"/>
-      <c r="GB1" s="16" t="s">
+      <c r="FA1" s="16"/>
+      <c r="FB1" s="16"/>
+      <c r="FC1" s="16"/>
+      <c r="FD1" s="16"/>
+      <c r="FE1" s="16"/>
+      <c r="FF1" s="16"/>
+      <c r="FG1" s="16"/>
+      <c r="FH1" s="16"/>
+      <c r="FI1" s="16"/>
+      <c r="FJ1" s="16"/>
+      <c r="FK1" s="16"/>
+      <c r="FL1" s="16"/>
+      <c r="FM1" s="16"/>
+      <c r="FN1" s="16"/>
+      <c r="FO1" s="16"/>
+      <c r="FP1" s="16"/>
+      <c r="FQ1" s="16"/>
+      <c r="FR1" s="16"/>
+      <c r="FS1" s="16"/>
+      <c r="FT1" s="16"/>
+      <c r="FU1" s="16"/>
+      <c r="FV1" s="16"/>
+      <c r="FW1" s="16"/>
+      <c r="FX1" s="16"/>
+      <c r="FY1" s="16"/>
+      <c r="FZ1" s="16"/>
+      <c r="GA1" s="16"/>
+      <c r="GB1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="GC1" s="14"/>
@@ -1260,37 +1205,37 @@
       <c r="HA1" s="14"/>
       <c r="HB1" s="14"/>
       <c r="HC1" s="14"/>
-      <c r="HD1" s="19" t="s">
+      <c r="HD1" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="HE1" s="17"/>
-      <c r="HF1" s="17"/>
-      <c r="HG1" s="17"/>
-      <c r="HH1" s="17"/>
-      <c r="HI1" s="17"/>
-      <c r="HJ1" s="17"/>
-      <c r="HK1" s="17"/>
-      <c r="HL1" s="17"/>
-      <c r="HM1" s="17"/>
-      <c r="HN1" s="17"/>
-      <c r="HO1" s="17"/>
-      <c r="HP1" s="17"/>
-      <c r="HQ1" s="17"/>
-      <c r="HR1" s="17"/>
-      <c r="HS1" s="17"/>
-      <c r="HT1" s="17"/>
-      <c r="HU1" s="17"/>
-      <c r="HV1" s="17"/>
-      <c r="HW1" s="17"/>
-      <c r="HX1" s="17"/>
-      <c r="HY1" s="17"/>
-      <c r="HZ1" s="17"/>
-      <c r="IA1" s="17"/>
-      <c r="IB1" s="17"/>
-      <c r="IC1" s="17"/>
-      <c r="ID1" s="17"/>
-      <c r="IE1" s="17"/>
-      <c r="IF1" s="16" t="s">
+      <c r="HE1" s="16"/>
+      <c r="HF1" s="16"/>
+      <c r="HG1" s="16"/>
+      <c r="HH1" s="16"/>
+      <c r="HI1" s="16"/>
+      <c r="HJ1" s="16"/>
+      <c r="HK1" s="16"/>
+      <c r="HL1" s="16"/>
+      <c r="HM1" s="16"/>
+      <c r="HN1" s="16"/>
+      <c r="HO1" s="16"/>
+      <c r="HP1" s="16"/>
+      <c r="HQ1" s="16"/>
+      <c r="HR1" s="16"/>
+      <c r="HS1" s="16"/>
+      <c r="HT1" s="16"/>
+      <c r="HU1" s="16"/>
+      <c r="HV1" s="16"/>
+      <c r="HW1" s="16"/>
+      <c r="HX1" s="16"/>
+      <c r="HY1" s="16"/>
+      <c r="HZ1" s="16"/>
+      <c r="IA1" s="16"/>
+      <c r="IB1" s="16"/>
+      <c r="IC1" s="16"/>
+      <c r="ID1" s="16"/>
+      <c r="IE1" s="16"/>
+      <c r="IF1" s="19" t="s">
         <v>79</v>
       </c>
       <c r="IG1" s="14"/>
@@ -1320,44 +1265,44 @@
       <c r="JE1" s="14"/>
       <c r="JF1" s="14"/>
       <c r="JG1" s="14"/>
-      <c r="JH1" s="12" t="s">
+      <c r="JH1" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="JI1" s="13"/>
-      <c r="JJ1" s="13"/>
-      <c r="JK1" s="13"/>
-      <c r="JL1" s="13"/>
-      <c r="JM1" s="13"/>
-      <c r="JN1" s="13"/>
-      <c r="JO1" s="13"/>
-      <c r="JP1" s="13"/>
-      <c r="JQ1" s="13"/>
-      <c r="JR1" s="13"/>
-      <c r="JS1" s="13"/>
-      <c r="JT1" s="13"/>
-      <c r="JU1" s="13"/>
-      <c r="JV1" s="13"/>
-      <c r="JW1" s="13"/>
-      <c r="JX1" s="13"/>
-      <c r="JY1" s="13"/>
-      <c r="JZ1" s="13"/>
-      <c r="KA1" s="13"/>
-      <c r="KB1" s="13"/>
-      <c r="KC1" s="13"/>
-      <c r="KD1" s="13"/>
-      <c r="KE1" s="13"/>
-      <c r="KF1" s="13"/>
-      <c r="KG1" s="13"/>
-      <c r="KH1" s="13"/>
-      <c r="KI1" s="13"/>
-      <c r="KJ1" s="13"/>
-      <c r="KK1" s="13"/>
-      <c r="KL1" s="13"/>
-      <c r="KM1" s="13"/>
-      <c r="KN1" s="13"/>
-      <c r="KO1" s="13"/>
-      <c r="KP1" s="13"/>
-      <c r="KQ1" s="13"/>
+      <c r="JI1" s="10"/>
+      <c r="JJ1" s="10"/>
+      <c r="JK1" s="10"/>
+      <c r="JL1" s="10"/>
+      <c r="JM1" s="10"/>
+      <c r="JN1" s="10"/>
+      <c r="JO1" s="10"/>
+      <c r="JP1" s="10"/>
+      <c r="JQ1" s="10"/>
+      <c r="JR1" s="10"/>
+      <c r="JS1" s="10"/>
+      <c r="JT1" s="10"/>
+      <c r="JU1" s="10"/>
+      <c r="JV1" s="10"/>
+      <c r="JW1" s="10"/>
+      <c r="JX1" s="10"/>
+      <c r="JY1" s="10"/>
+      <c r="JZ1" s="10"/>
+      <c r="KA1" s="10"/>
+      <c r="KB1" s="10"/>
+      <c r="KC1" s="10"/>
+      <c r="KD1" s="10"/>
+      <c r="KE1" s="10"/>
+      <c r="KF1" s="10"/>
+      <c r="KG1" s="10"/>
+      <c r="KH1" s="10"/>
+      <c r="KI1" s="10"/>
+      <c r="KJ1" s="10"/>
+      <c r="KK1" s="10"/>
+      <c r="KL1" s="10"/>
+      <c r="KM1" s="10"/>
+      <c r="KN1" s="10"/>
+      <c r="KO1" s="10"/>
+      <c r="KP1" s="10"/>
+      <c r="KQ1" s="10"/>
     </row>
     <row r="2" spans="1:303" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -1496,46 +1441,46 @@
         <v>49</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>51</v>
+        <v>149</v>
       </c>
       <c r="AV2" s="3" t="s">
-        <v>52</v>
+        <v>150</v>
       </c>
       <c r="AW2" s="3" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="AX2" s="3" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="AY2" s="3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="AZ2" s="3" t="s">
-        <v>56</v>
+        <v>151</v>
       </c>
       <c r="BA2" s="3" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="BB2" s="3" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="BC2" s="3" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="BD2" s="3" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="BE2" s="3" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="BF2" s="3" t="s">
-        <v>60</v>
+        <v>152</v>
       </c>
       <c r="BG2" s="3" t="s">
-        <v>61</v>
+        <v>153</v>
       </c>
       <c r="BH2" s="3" t="s">
         <v>62</v>
@@ -1580,46 +1525,46 @@
         <v>49</v>
       </c>
       <c r="BV2" s="15" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="BW2" s="15" t="s">
-        <v>51</v>
+        <v>149</v>
       </c>
       <c r="BX2" s="15" t="s">
-        <v>52</v>
+        <v>150</v>
       </c>
       <c r="BY2" s="15" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="BZ2" s="15" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="CA2" s="15" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="CB2" s="15" t="s">
-        <v>56</v>
+        <v>151</v>
       </c>
       <c r="CC2" s="15" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="CD2" s="15" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="CE2" s="15" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="CF2" s="15" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="CG2" s="15" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="CH2" s="15" t="s">
-        <v>60</v>
+        <v>152</v>
       </c>
       <c r="CI2" s="15" t="s">
-        <v>61</v>
+        <v>153</v>
       </c>
       <c r="CJ2" s="15" t="s">
         <v>62</v>
@@ -1657,88 +1602,88 @@
       <c r="CU2" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="CV2" s="18" t="s">
+      <c r="CV2" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="CW2" s="18" t="s">
+      <c r="CW2" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="CX2" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="CY2" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="CZ2" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="DA2" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="DB2" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="DC2" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="DD2" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="DE2" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="DF2" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="DG2" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="DH2" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="DI2" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="DJ2" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="DK2" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="DL2" s="18" t="s">
+      <c r="CX2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="CY2" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="CZ2" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="DA2" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="DB2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="DC2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="DD2" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="DE2" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="DF2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="DG2" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="DH2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="DI2" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="DJ2" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="DK2" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="DL2" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="DM2" s="18" t="s">
+      <c r="DM2" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="DN2" s="18" t="s">
+      <c r="DN2" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="DO2" s="18" t="s">
+      <c r="DO2" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="DP2" s="18" t="s">
+      <c r="DP2" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="DQ2" s="18" t="s">
+      <c r="DQ2" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="DR2" s="18" t="s">
+      <c r="DR2" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="DS2" s="18" t="s">
+      <c r="DS2" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="DT2" s="18" t="s">
+      <c r="DT2" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="DU2" s="18" t="s">
+      <c r="DU2" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="DV2" s="18" t="s">
+      <c r="DV2" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="DW2" s="18" t="s">
+      <c r="DW2" s="17" t="s">
         <v>93</v>
       </c>
       <c r="DX2" s="15" t="s">
@@ -1748,46 +1693,46 @@
         <v>49</v>
       </c>
       <c r="DZ2" s="15" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="EA2" s="15" t="s">
-        <v>51</v>
+        <v>149</v>
       </c>
       <c r="EB2" s="15" t="s">
-        <v>52</v>
+        <v>150</v>
       </c>
       <c r="EC2" s="15" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="ED2" s="15" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="EE2" s="15" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="EF2" s="15" t="s">
-        <v>56</v>
+        <v>151</v>
       </c>
       <c r="EG2" s="15" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="EH2" s="15" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="EI2" s="15" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="EJ2" s="15" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="EK2" s="15" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="EL2" s="15" t="s">
-        <v>60</v>
+        <v>152</v>
       </c>
       <c r="EM2" s="15" t="s">
-        <v>61</v>
+        <v>153</v>
       </c>
       <c r="EN2" s="15" t="s">
         <v>62</v>
@@ -1825,88 +1770,88 @@
       <c r="EY2" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="EZ2" s="18" t="s">
+      <c r="EZ2" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="FA2" s="18" t="s">
+      <c r="FA2" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="FB2" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="FC2" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="FD2" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="FE2" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="FF2" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="FG2" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="FH2" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="FI2" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="FJ2" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="FK2" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="FL2" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="FM2" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="FN2" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="FO2" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="FP2" s="18" t="s">
+      <c r="FB2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="FC2" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="FD2" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="FE2" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="FF2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="FG2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="FH2" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="FI2" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="FJ2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="FK2" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="FL2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="FM2" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="FN2" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="FO2" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="FP2" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="FQ2" s="18" t="s">
+      <c r="FQ2" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="FR2" s="18" t="s">
+      <c r="FR2" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="FS2" s="18" t="s">
+      <c r="FS2" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="FT2" s="18" t="s">
+      <c r="FT2" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="FU2" s="18" t="s">
+      <c r="FU2" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="FV2" s="18" t="s">
+      <c r="FV2" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="FW2" s="18" t="s">
+      <c r="FW2" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="FX2" s="18" t="s">
+      <c r="FX2" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="FY2" s="18" t="s">
+      <c r="FY2" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="FZ2" s="18" t="s">
+      <c r="FZ2" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="GA2" s="18" t="s">
+      <c r="GA2" s="17" t="s">
         <v>93</v>
       </c>
       <c r="GB2" s="15" t="s">
@@ -1916,46 +1861,46 @@
         <v>49</v>
       </c>
       <c r="GD2" s="15" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="GE2" s="15" t="s">
-        <v>51</v>
+        <v>149</v>
       </c>
       <c r="GF2" s="15" t="s">
-        <v>52</v>
+        <v>150</v>
       </c>
       <c r="GG2" s="15" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="GH2" s="15" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="GI2" s="15" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="GJ2" s="15" t="s">
-        <v>56</v>
+        <v>151</v>
       </c>
       <c r="GK2" s="15" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="GL2" s="15" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="GM2" s="15" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="GN2" s="15" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="GO2" s="15" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="GP2" s="15" t="s">
-        <v>60</v>
+        <v>152</v>
       </c>
       <c r="GQ2" s="15" t="s">
-        <v>61</v>
+        <v>153</v>
       </c>
       <c r="GR2" s="15" t="s">
         <v>62</v>
@@ -1993,88 +1938,88 @@
       <c r="HC2" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="HD2" s="18" t="s">
+      <c r="HD2" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="HE2" s="18" t="s">
+      <c r="HE2" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="HF2" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="HG2" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="HH2" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="HI2" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="HJ2" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="HK2" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="HL2" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="HM2" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="HN2" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="HO2" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="HP2" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="HQ2" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="HR2" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="HS2" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="HT2" s="18" t="s">
+      <c r="HF2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="HG2" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="HH2" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="HI2" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="HJ2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="HK2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="HL2" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="HM2" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="HN2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="HO2" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="HP2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="HQ2" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="HR2" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="HS2" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="HT2" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="HU2" s="18" t="s">
+      <c r="HU2" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="HV2" s="18" t="s">
+      <c r="HV2" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="HW2" s="18" t="s">
+      <c r="HW2" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="HX2" s="18" t="s">
+      <c r="HX2" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="HY2" s="18" t="s">
+      <c r="HY2" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="HZ2" s="18" t="s">
+      <c r="HZ2" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="IA2" s="18" t="s">
+      <c r="IA2" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="IB2" s="18" t="s">
+      <c r="IB2" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="IC2" s="18" t="s">
+      <c r="IC2" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="ID2" s="18" t="s">
+      <c r="ID2" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="IE2" s="18" t="s">
+      <c r="IE2" s="17" t="s">
         <v>93</v>
       </c>
       <c r="IF2" s="15" t="s">
@@ -2084,46 +2029,46 @@
         <v>49</v>
       </c>
       <c r="IH2" s="15" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="II2" s="15" t="s">
-        <v>51</v>
+        <v>149</v>
       </c>
       <c r="IJ2" s="15" t="s">
-        <v>52</v>
+        <v>150</v>
       </c>
       <c r="IK2" s="15" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="IL2" s="15" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="IM2" s="15" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="IN2" s="15" t="s">
-        <v>56</v>
+        <v>151</v>
       </c>
       <c r="IO2" s="15" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="IP2" s="15" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="IQ2" s="15" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="IR2" s="15" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="IS2" s="15" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="IT2" s="15" t="s">
-        <v>60</v>
+        <v>152</v>
       </c>
       <c r="IU2" s="15" t="s">
-        <v>61</v>
+        <v>153</v>
       </c>
       <c r="IV2" s="15" t="s">
         <v>62</v>
@@ -2269,23 +2214,539 @@
       <c r="KQ2" s="7" t="s">
         <v>70</v>
       </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J3" t="s">
+        <v>103</v>
+      </c>
+      <c r="K3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L3" t="s">
+        <v>105</v>
+      </c>
+      <c r="M3" t="s">
+        <v>106</v>
+      </c>
+      <c r="N3" t="s">
+        <v>107</v>
+      </c>
+      <c r="O3" t="s">
+        <v>106</v>
+      </c>
+      <c r="P3" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>109</v>
+      </c>
+      <c r="R3" t="s">
+        <v>110</v>
+      </c>
+      <c r="S3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T3" t="s">
+        <v>111</v>
+      </c>
+      <c r="U3" t="s">
+        <v>105</v>
+      </c>
+      <c r="V3" t="s">
+        <v>112</v>
+      </c>
+      <c r="W3" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>120</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>123</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>124</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>108</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>111</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>123</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>125</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>105</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>108</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>124</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>105</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>126</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>127</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>126</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>105</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>125</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>127</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>126</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>128</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>105</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>129</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>105</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>130</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>131</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>104</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>110</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>122</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>104</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>110</v>
+      </c>
+      <c r="CB3" t="s">
+        <v>124</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>110</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>132</v>
+      </c>
+      <c r="CE3" t="s">
+        <v>115</v>
+      </c>
+      <c r="CF3" t="s">
+        <v>108</v>
+      </c>
+      <c r="CG3" t="s">
+        <v>124</v>
+      </c>
+      <c r="CH3" t="s">
+        <v>132</v>
+      </c>
+      <c r="CI3" t="s">
+        <v>132</v>
+      </c>
+      <c r="CJ3" t="s">
+        <v>126</v>
+      </c>
+      <c r="CK3" t="s">
+        <v>125</v>
+      </c>
+      <c r="CL3" t="s">
+        <v>125</v>
+      </c>
+      <c r="CM3" t="s">
+        <v>126</v>
+      </c>
+      <c r="CN3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CO3" t="s">
+        <v>105</v>
+      </c>
+      <c r="CP3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CQ3" t="s">
+        <v>127</v>
+      </c>
+      <c r="CR3" t="s">
+        <v>126</v>
+      </c>
+      <c r="CS3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CT3" t="s">
+        <v>127</v>
+      </c>
+      <c r="CU3" t="s">
+        <v>134</v>
+      </c>
+      <c r="CV3"/>
+      <c r="JH3" t="s">
+        <v>135</v>
+      </c>
+      <c r="JI3" t="s">
+        <v>127</v>
+      </c>
+      <c r="JJ3" t="s">
+        <v>108</v>
+      </c>
+      <c r="JK3" t="s">
+        <v>110</v>
+      </c>
+      <c r="JL3" t="s">
+        <v>124</v>
+      </c>
+      <c r="JM3" t="s">
+        <v>111</v>
+      </c>
+      <c r="JN3" t="s">
+        <v>136</v>
+      </c>
+      <c r="JO3" t="s">
+        <v>111</v>
+      </c>
+      <c r="JP3" t="s">
+        <v>137</v>
+      </c>
+      <c r="JQ3" t="s">
+        <v>111</v>
+      </c>
+      <c r="JR3" t="s">
+        <v>127</v>
+      </c>
+      <c r="JS3" t="s">
+        <v>123</v>
+      </c>
+      <c r="JT3" t="s">
+        <v>110</v>
+      </c>
+      <c r="JU3" t="s">
+        <v>105</v>
+      </c>
+      <c r="JV3" t="s">
+        <v>132</v>
+      </c>
+      <c r="JW3" t="s">
+        <v>105</v>
+      </c>
+      <c r="JX3" t="s">
+        <v>121</v>
+      </c>
+      <c r="JY3" t="s">
+        <v>108</v>
+      </c>
+      <c r="JZ3" t="s">
+        <v>45</v>
+      </c>
+      <c r="KA3" t="s">
+        <v>138</v>
+      </c>
+      <c r="KB3" t="s">
+        <v>132</v>
+      </c>
+      <c r="KC3" t="s">
+        <v>139</v>
+      </c>
+      <c r="KD3" t="s">
+        <v>140</v>
+      </c>
+      <c r="KE3"/>
+      <c r="KF3"/>
+      <c r="KG3"/>
+      <c r="KH3"/>
+      <c r="KI3"/>
+      <c r="KJ3"/>
+      <c r="KK3"/>
+      <c r="KL3"/>
+      <c r="KM3"/>
+      <c r="KN3"/>
+      <c r="KO3"/>
+      <c r="KP3"/>
+      <c r="KQ3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H4" t="s">
+        <v>118</v>
+      </c>
+      <c r="I4" t="s">
+        <v>148</v>
+      </c>
+      <c r="J4" t="s">
+        <v>132</v>
+      </c>
+      <c r="K4" t="s">
+        <v>108</v>
+      </c>
+      <c r="L4" t="s">
+        <v>105</v>
+      </c>
+      <c r="M4" t="s">
+        <v>106</v>
+      </c>
+      <c r="N4" t="s">
+        <v>107</v>
+      </c>
+      <c r="O4" t="s">
+        <v>106</v>
+      </c>
+      <c r="P4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>109</v>
+      </c>
+      <c r="R4" t="s">
+        <v>110</v>
+      </c>
+      <c r="S4" t="s">
+        <v>110</v>
+      </c>
+      <c r="T4" t="s">
+        <v>108</v>
+      </c>
+      <c r="U4" t="s">
+        <v>132</v>
+      </c>
+      <c r="V4" t="s">
+        <v>110</v>
+      </c>
+      <c r="W4" t="s">
+        <v>46</v>
+      </c>
+      <c r="X4" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>124</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>125</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>132</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>124</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>136</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AR4"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="BT1:CU1"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="J1:AQ1"/>
+    <mergeCell ref="AR1:BS1"/>
+    <mergeCell ref="CV1:DW1"/>
     <mergeCell ref="JH1:KQ1"/>
     <mergeCell ref="DX1:EY1"/>
     <mergeCell ref="EZ1:GA1"/>
     <mergeCell ref="GB1:HC1"/>
     <mergeCell ref="HD1:IE1"/>
     <mergeCell ref="IF1:JG1"/>
-    <mergeCell ref="BT1:CU1"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="J1:AQ1"/>
-    <mergeCell ref="AR1:BS1"/>
-    <mergeCell ref="CV1:DW1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <ignoredErrors>
+    <ignoredError sqref="CT3" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correccion bug 3. Parte1.
</commit_message>
<xml_diff>
--- a/formato.xlsx
+++ b/formato.xlsx
@@ -2215,520 +2215,6 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H3" t="s">
-        <v>101</v>
-      </c>
-      <c r="I3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J3" t="s">
-        <v>103</v>
-      </c>
-      <c r="K3" t="s">
-        <v>104</v>
-      </c>
-      <c r="L3" t="s">
-        <v>105</v>
-      </c>
-      <c r="M3" t="s">
-        <v>106</v>
-      </c>
-      <c r="N3" t="s">
-        <v>107</v>
-      </c>
-      <c r="O3" t="s">
-        <v>106</v>
-      </c>
-      <c r="P3" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>109</v>
-      </c>
-      <c r="R3" t="s">
-        <v>110</v>
-      </c>
-      <c r="S3" t="s">
-        <v>110</v>
-      </c>
-      <c r="T3" t="s">
-        <v>111</v>
-      </c>
-      <c r="U3" t="s">
-        <v>105</v>
-      </c>
-      <c r="V3" t="s">
-        <v>112</v>
-      </c>
-      <c r="W3" t="s">
-        <v>45</v>
-      </c>
-      <c r="X3" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>114</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>115</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>106</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>109</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>112</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>101</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>114</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>118</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>109</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>109</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>106</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>107</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>119</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>121</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>108</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>122</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>123</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>124</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>108</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>111</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>123</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>125</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>105</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>108</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>124</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>107</v>
-      </c>
-      <c r="BI3" t="s">
-        <v>105</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>126</v>
-      </c>
-      <c r="BK3" t="s">
-        <v>127</v>
-      </c>
-      <c r="BL3" t="s">
-        <v>126</v>
-      </c>
-      <c r="BM3" t="s">
-        <v>105</v>
-      </c>
-      <c r="BN3" t="s">
-        <v>125</v>
-      </c>
-      <c r="BO3" t="s">
-        <v>127</v>
-      </c>
-      <c r="BP3" t="s">
-        <v>126</v>
-      </c>
-      <c r="BQ3" t="s">
-        <v>128</v>
-      </c>
-      <c r="BR3" t="s">
-        <v>105</v>
-      </c>
-      <c r="BS3" t="s">
-        <v>129</v>
-      </c>
-      <c r="BT3" t="s">
-        <v>105</v>
-      </c>
-      <c r="BU3" t="s">
-        <v>130</v>
-      </c>
-      <c r="BV3" t="s">
-        <v>131</v>
-      </c>
-      <c r="BW3" t="s">
-        <v>104</v>
-      </c>
-      <c r="BX3" t="s">
-        <v>110</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>122</v>
-      </c>
-      <c r="BZ3" t="s">
-        <v>104</v>
-      </c>
-      <c r="CA3" t="s">
-        <v>110</v>
-      </c>
-      <c r="CB3" t="s">
-        <v>124</v>
-      </c>
-      <c r="CC3" t="s">
-        <v>110</v>
-      </c>
-      <c r="CD3" t="s">
-        <v>132</v>
-      </c>
-      <c r="CE3" t="s">
-        <v>115</v>
-      </c>
-      <c r="CF3" t="s">
-        <v>108</v>
-      </c>
-      <c r="CG3" t="s">
-        <v>124</v>
-      </c>
-      <c r="CH3" t="s">
-        <v>132</v>
-      </c>
-      <c r="CI3" t="s">
-        <v>132</v>
-      </c>
-      <c r="CJ3" t="s">
-        <v>126</v>
-      </c>
-      <c r="CK3" t="s">
-        <v>125</v>
-      </c>
-      <c r="CL3" t="s">
-        <v>125</v>
-      </c>
-      <c r="CM3" t="s">
-        <v>126</v>
-      </c>
-      <c r="CN3" t="s">
-        <v>107</v>
-      </c>
-      <c r="CO3" t="s">
-        <v>105</v>
-      </c>
-      <c r="CP3" t="s">
-        <v>107</v>
-      </c>
-      <c r="CQ3" t="s">
-        <v>127</v>
-      </c>
-      <c r="CR3" t="s">
-        <v>126</v>
-      </c>
-      <c r="CS3" t="s">
-        <v>133</v>
-      </c>
-      <c r="CT3" t="s">
-        <v>127</v>
-      </c>
-      <c r="CU3" t="s">
-        <v>134</v>
-      </c>
-      <c r="CV3"/>
-      <c r="JH3" t="s">
-        <v>135</v>
-      </c>
-      <c r="JI3" t="s">
-        <v>127</v>
-      </c>
-      <c r="JJ3" t="s">
-        <v>108</v>
-      </c>
-      <c r="JK3" t="s">
-        <v>110</v>
-      </c>
-      <c r="JL3" t="s">
-        <v>124</v>
-      </c>
-      <c r="JM3" t="s">
-        <v>111</v>
-      </c>
-      <c r="JN3" t="s">
-        <v>136</v>
-      </c>
-      <c r="JO3" t="s">
-        <v>111</v>
-      </c>
-      <c r="JP3" t="s">
-        <v>137</v>
-      </c>
-      <c r="JQ3" t="s">
-        <v>111</v>
-      </c>
-      <c r="JR3" t="s">
-        <v>127</v>
-      </c>
-      <c r="JS3" t="s">
-        <v>123</v>
-      </c>
-      <c r="JT3" t="s">
-        <v>110</v>
-      </c>
-      <c r="JU3" t="s">
-        <v>105</v>
-      </c>
-      <c r="JV3" t="s">
-        <v>132</v>
-      </c>
-      <c r="JW3" t="s">
-        <v>105</v>
-      </c>
-      <c r="JX3" t="s">
-        <v>121</v>
-      </c>
-      <c r="JY3" t="s">
-        <v>108</v>
-      </c>
-      <c r="JZ3" t="s">
-        <v>45</v>
-      </c>
-      <c r="KA3" t="s">
-        <v>138</v>
-      </c>
-      <c r="KB3" t="s">
-        <v>132</v>
-      </c>
-      <c r="KC3" t="s">
-        <v>139</v>
-      </c>
-      <c r="KD3" t="s">
-        <v>140</v>
-      </c>
-      <c r="KE3"/>
-      <c r="KF3"/>
-      <c r="KG3"/>
-      <c r="KH3"/>
-      <c r="KI3"/>
-      <c r="KJ3"/>
-      <c r="KK3"/>
-      <c r="KL3"/>
-      <c r="KM3"/>
-      <c r="KN3"/>
-      <c r="KO3"/>
-      <c r="KP3"/>
-      <c r="KQ3"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F4" t="s">
-        <v>146</v>
-      </c>
-      <c r="G4" t="s">
-        <v>147</v>
-      </c>
-      <c r="H4" t="s">
-        <v>118</v>
-      </c>
-      <c r="I4" t="s">
-        <v>148</v>
-      </c>
-      <c r="J4" t="s">
-        <v>132</v>
-      </c>
-      <c r="K4" t="s">
-        <v>108</v>
-      </c>
-      <c r="L4" t="s">
-        <v>105</v>
-      </c>
-      <c r="M4" t="s">
-        <v>106</v>
-      </c>
-      <c r="N4" t="s">
-        <v>107</v>
-      </c>
-      <c r="O4" t="s">
-        <v>106</v>
-      </c>
-      <c r="P4" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>109</v>
-      </c>
-      <c r="R4" t="s">
-        <v>110</v>
-      </c>
-      <c r="S4" t="s">
-        <v>110</v>
-      </c>
-      <c r="T4" t="s">
-        <v>108</v>
-      </c>
-      <c r="U4" t="s">
-        <v>132</v>
-      </c>
-      <c r="V4" t="s">
-        <v>110</v>
-      </c>
-      <c r="W4" t="s">
-        <v>46</v>
-      </c>
-      <c r="X4" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>132</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>125</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>108</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>109</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>109</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>124</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>125</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>132</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>124</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>136</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>137</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>109</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>109</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>109</v>
-      </c>
-      <c r="AR4"/>
-    </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="BT1:CU1"/>

</xml_diff>

<commit_message>
Issue delete docotor fixed.
</commit_message>
<xml_diff>
--- a/formato.xlsx
+++ b/formato.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="174">
   <si>
     <t>Nombre</t>
   </si>
@@ -487,6 +487,66 @@
   </si>
   <si>
     <t>Cadenas Ligeras Lambda (mg/dL)</t>
+  </si>
+  <si>
+    <t>Adriana Hernandez Caballero</t>
+  </si>
+  <si>
+    <t>1978-09-07</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>168</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>1.65 m²</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Julio Juarez Mendoza</t>
+  </si>
+  <si>
+    <t>1984-06-14</t>
+  </si>
+  <si>
+    <t>2017-06-08</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>2.1 m²</t>
+  </si>
+  <si>
+    <t>No secretor</t>
+  </si>
+  <si>
+    <t>Eduardo Rosas Lopez</t>
+  </si>
+  <si>
+    <t>1985-06-04</t>
+  </si>
+  <si>
+    <t>2010-06-08</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>2.21 m²</t>
   </si>
 </sst>
 </file>
@@ -2215,6 +2275,402 @@
         <v>70</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H3" t="s">
+        <v>158</v>
+      </c>
+      <c r="I3" t="s">
+        <v>159</v>
+      </c>
+      <c r="J3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K3" t="s">
+        <v>122</v>
+      </c>
+      <c r="L3" t="s">
+        <v>105</v>
+      </c>
+      <c r="M3" t="s">
+        <v>109</v>
+      </c>
+      <c r="N3" t="s">
+        <v>160</v>
+      </c>
+      <c r="O3" t="s">
+        <v>109</v>
+      </c>
+      <c r="P3" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>109</v>
+      </c>
+      <c r="R3" t="s">
+        <v>111</v>
+      </c>
+      <c r="S3" t="s">
+        <v>104</v>
+      </c>
+      <c r="T3" t="s">
+        <v>127</v>
+      </c>
+      <c r="U3" t="s">
+        <v>122</v>
+      </c>
+      <c r="V3" t="s">
+        <v>110</v>
+      </c>
+      <c r="W3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>124</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AR3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G4" t="s">
+        <v>164</v>
+      </c>
+      <c r="H4" t="s">
+        <v>165</v>
+      </c>
+      <c r="I4" t="s">
+        <v>166</v>
+      </c>
+      <c r="J4" t="s">
+        <v>124</v>
+      </c>
+      <c r="K4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" t="s">
+        <v>107</v>
+      </c>
+      <c r="M4" t="s">
+        <v>106</v>
+      </c>
+      <c r="N4" t="s">
+        <v>160</v>
+      </c>
+      <c r="O4" t="s">
+        <v>106</v>
+      </c>
+      <c r="P4" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>109</v>
+      </c>
+      <c r="R4" t="s">
+        <v>111</v>
+      </c>
+      <c r="S4" t="s">
+        <v>108</v>
+      </c>
+      <c r="T4" t="s">
+        <v>111</v>
+      </c>
+      <c r="U4" t="s">
+        <v>104</v>
+      </c>
+      <c r="V4" t="s">
+        <v>110</v>
+      </c>
+      <c r="W4" t="s">
+        <v>46</v>
+      </c>
+      <c r="X4" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>124</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>124</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AR4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F5" t="s">
+        <v>146</v>
+      </c>
+      <c r="G5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H5" t="s">
+        <v>172</v>
+      </c>
+      <c r="I5" t="s">
+        <v>173</v>
+      </c>
+      <c r="J5" t="s">
+        <v>124</v>
+      </c>
+      <c r="K5" t="s">
+        <v>122</v>
+      </c>
+      <c r="L5" t="s">
+        <v>105</v>
+      </c>
+      <c r="M5" t="s">
+        <v>109</v>
+      </c>
+      <c r="N5" t="s">
+        <v>160</v>
+      </c>
+      <c r="O5" t="s">
+        <v>106</v>
+      </c>
+      <c r="P5" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>109</v>
+      </c>
+      <c r="R5" t="s">
+        <v>110</v>
+      </c>
+      <c r="S5" t="s">
+        <v>125</v>
+      </c>
+      <c r="T5" t="s">
+        <v>127</v>
+      </c>
+      <c r="U5" t="s">
+        <v>127</v>
+      </c>
+      <c r="V5" t="s">
+        <v>112</v>
+      </c>
+      <c r="W5" t="s">
+        <v>46</v>
+      </c>
+      <c r="X5" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>132</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>124</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>124</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>111</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>111</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>109</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>106</v>
+      </c>
+      <c r="AR5"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="BT1:CU1"/>

</xml_diff>